<commit_message>
finish What is unique Airbnb? section
</commit_message>
<xml_diff>
--- a/review_sample.xlsx
+++ b/review_sample.xlsx
@@ -29,27 +29,22 @@
     <t>type</t>
   </si>
   <si>
-    <t>Superbe Séjour, appartement conforme aux photos. Proximité du métro. Quartier sans problèmes. Maba est très sympathique, disponible et très réactif en cas de besoin. Petit bémol sur la propreté du sol de l’appartement et les chaines Tv US ne sont pas disponibles (uniquement Netflix, Hulu ... Une adresse où séjourner sans hésiter. Merci MABA</t>
+    <t xml:space="preserve">Vitaliy provided very informative directions and instructions on getting into the apartment. The apartment was exactly like it was in the photos. Harlem is a unique neighbourhood in NYC and will give you a different flavour of the city. </t>
   </si>
   <si>
     <t>"unique" review</t>
   </si>
   <si>
-    <t>great stay in a super convenient location. beach, restaurants, and more all within a ten minute walk. the studio is rather small, but for just two people it was perfect (especially if you’re not planning on spending most of the day inside). would definitely stay here again!</t>
-  </si>
-  <si>
-    <t>You are going to love this place!
-Not only is Kate’s brownstone super cute but the location is perfect! 
-Close to everything you need (Trader Joe’s my fav)and easy commute into Manhattan. 
-Super accommodating and quick to respond to any questions. 
-Definitely will recommend.
-Thanks again Kate!</t>
+    <t>The location of this apartment is great - very close to the subway and it allows you to reach Manhattan quickly. Good restaurants in the neighborhood. Maxime's (Hidden by Airbnb) , who were at home when we stayed, were absolutely fantastic and they made our experience in NYC special.</t>
+  </si>
+  <si>
+    <t>A rather cool yet inviting &amp; comfortable place.  We felt like we had our own little nest in the big city!❤️</t>
   </si>
   <si>
     <t>"non-unique" review</t>
   </si>
   <si>
-    <t>Beautiful place!! Smelled amazed. Felt like a home away from home.</t>
+    <t>Einfach nur empfehlenswert!!!</t>
   </si>
 </sst>
 </file>
@@ -426,10 +421,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="n">
-        <v>14092239</v>
+        <v>9576478</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>43048</v>
+        <v>42615</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -440,10 +435,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="n">
-        <v>37592568</v>
+        <v>27930717</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44066</v>
+        <v>43347</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -454,10 +449,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="n">
-        <v>19226317</v>
+        <v>13192097</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>43831</v>
+        <v>43524</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -468,10 +463,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="n">
-        <v>25042316</v>
+        <v>18803064</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44015</v>
+        <v>43411</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>

</xml_diff>